<commit_message>
Remove targets do schema para campos permanecerem com os nomes utilizados na geração do volume 7 da LOA.
</commit_message>
<xml_diff>
--- a/data/base_qdd_fiscal_fonte_95.xlsx
+++ b/data/base_qdd_fiscal_fonte_95.xlsx
@@ -7275,6 +7275,11 @@
       <c r="Y60" t="n">
         <v>0</v>
       </c>
+      <c r="Z60" t="inlineStr">
+        <is>
+          <t>PROTEÇÃO E CONSERVAÇÃO DA FAUNA SILVESTRE</t>
+        </is>
+      </c>
       <c r="AA60" t="inlineStr">
         <is>
           <t>PROTEÇÃO DAS ÁREAS AMBIENTALMENTE CONSERVADAS, DA FAUNA E DA BIODIVERSIDADE FLORESTAL</t>

</xml_diff>

<commit_message>
Update data package at: 2024-09-26T18:56:28Z
</commit_message>
<xml_diff>
--- a/data/base_qdd_fiscal_fonte_95.xlsx
+++ b/data/base_qdd_fiscal_fonte_95.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH39"/>
+  <dimension ref="A1:AF39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
@@ -578,16 +578,6 @@
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>Observações</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>NOVO NOME</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
           <t>ESPECIFICAÇÃO</t>
         </is>
       </c>
@@ -615,7 +605,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SECRETARIA DE ESTADO DE AGRICULTURA, PECUÁRIA E ABASTECIMENTO - SEAPA - SEAPA</t>
+          <t>SECRETARIA DE ESTADO DE AGRICULTURA, PECUÁRIA E ABASTECIMENTO - SEAPA</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -689,12 +679,12 @@
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
@@ -702,14 +692,9 @@
           <t>Atualização e realização de novos estudos de Zoneamento Ambiental Produtivo em sub-bacias hidrográficas da bacia do rio Doce</t>
         </is>
       </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>Atualização e realização de novos estudos de Zoneamento Ambiental Produtivo em sub-bacias hidrográficas da bacia do rio Doce</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Atualização e realização de novos estudos de Zoneamento Ambiental Produtivo em sub-bacias hidrográficas da bacia do rio Doce</t>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Atualização e realização de novos estudos de Zoneamento Ambiental Produtivo em sub-bacias hidrográficas da bacia do rio Doce</t>
         </is>
       </c>
     </row>
@@ -810,12 +795,12 @@
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
@@ -825,21 +810,28 @@
       </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t>Valor bem maior que o solicitado mas o total fecha (!)</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>Ações de Reposta a Enchentes e de Recuperação Ambiental e Produtiva das Margens do rio Doce</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Ações de Reposta a Enchentes e de Recuperação Ambiental e Produtiva das Margens do rio Doce</t>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Ações de Reposta a Enchentes e de Recuperação Ambiental e Produtiva das Margens do rio Doce</t>
         </is>
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1230</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SECRETARIA DE ESTADO DE AGRICULTURA, PECUÁRIA E ABASTECIMENTO - SEAPA</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
       <c r="F4" t="n">
         <v>3041</v>
       </c>
@@ -919,12 +911,12 @@
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
@@ -934,21 +926,28 @@
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>Complementei com os outros 2 projetos EMATER que já constavam na listagem</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>Realização de diagnóstico dos pescadores da região para guiar ações de capacitação para a atividade rural e instalação de unidades produtivas de criação de peixes em tanque e assistência técnica para sua utilização</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Realização de diagnóstico dos pescadores da região para guiar ações de capacitação para a atividade rural e instalação de unidades produtivas de criação de peixes em tanque e assistência técnica para sua utilização</t>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Realização de diagnóstico dos pescadores da região para guiar ações de capacitação para a atividade rural e instalação de unidades produtivas de criação de peixes em tanque e assistência técnica para sua utilização</t>
         </is>
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1230</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SECRETARIA DE ESTADO DE AGRICULTURA, PECUÁRIA E ABASTECIMENTO - SEAPA</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
       <c r="F5" t="n">
         <v>3041</v>
       </c>
@@ -1028,12 +1027,12 @@
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
@@ -1043,17 +1042,7 @@
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>Complementei com os outros 2 projetos EMATER que já constavam na listagem</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>Oferta de serviços de assistência técnica e extensão rural (metodologia ISA/PASEA), visando à produção de alimentos e estímulo à comercialização e adequação socioeconômica e ambiental de propriedades rurais</t>
-        </is>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Oferta de serviços de assistência técnica e extensão rural (metodologia ISA/PASEA), visando à produção de alimentos e estímulo à comercialização e adequação socioeconômica e ambiental de propriedades rurais</t>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Oferta de serviços de assistência técnica e extensão rural (metodologia ISA/PASEA), visando à produção de alimentos e estímulo à comercialização e adequação socioeconômica e ambiental de propriedades rurais</t>
         </is>
       </c>
     </row>
@@ -1154,32 +1143,22 @@
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG </t>
+          <t>Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>Valor da PM ficou a mais do que o final (não autorizado a mudar). Deixei o valor total da base Mariana e o resto no geral</t>
-        </is>
-      </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
-        </is>
-      </c>
-      <c r="AH6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Acordo Repactuação Rio Doce - N/A - A cadastrar - Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG </t>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
         </is>
       </c>
     </row>
@@ -1227,6 +1206,24 @@
       <c r="M7" t="n">
         <v>1</v>
       </c>
+      <c r="N7" t="n">
+        <v>10690</v>
+      </c>
+      <c r="O7" t="n">
+        <v>6</v>
+      </c>
+      <c r="P7" t="n">
+        <v>181</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>137</v>
+      </c>
+      <c r="R7" t="n">
+        <v>4</v>
+      </c>
+      <c r="S7" t="n">
+        <v>365</v>
+      </c>
       <c r="T7" t="n">
         <v>4365</v>
       </c>
@@ -1234,19 +1231,27 @@
         <v>1</v>
       </c>
       <c r="V7" t="n">
-        <v>4796778.06</v>
+        <v>4796778</v>
       </c>
       <c r="W7" t="n">
-        <v>4796778.06</v>
+        <v>4796778</v>
       </c>
       <c r="X7" t="n">
         <v>4796778</v>
       </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
       <c r="Z7" t="inlineStr">
         <is>
           <t>POLICIAMENTO OSTENSIVO GERAL</t>
         </is>
       </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>POLÍCIA OSTENSIVA</t>
+        </is>
+      </c>
       <c r="AB7" t="inlineStr">
         <is>
           <t>Acordo Repactuação Rio Doce</t>
@@ -1254,36 +1259,43 @@
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG </t>
+          <t>Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>Valor da PM ficou a mais do que o final (não autorizado a mudar). Deixei o valor total da base Mariana e o resto no geral</t>
-        </is>
-      </c>
-      <c r="AG7" t="inlineStr">
-        <is>
-          <t>Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
-        </is>
-      </c>
-      <c r="AH7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Acordo Repactuação Rio Doce - N/A - A cadastrar - Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG </t>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
         </is>
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1250</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>POLÍCIA MILITAR DO ESTADO DE MINAS GERAIS - PMMG</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
       <c r="F8" t="n">
         <v>1251</v>
       </c>
@@ -1310,6 +1322,24 @@
       <c r="M8" t="n">
         <v>1</v>
       </c>
+      <c r="N8" t="n">
+        <v>10690</v>
+      </c>
+      <c r="O8" t="n">
+        <v>6</v>
+      </c>
+      <c r="P8" t="n">
+        <v>181</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>137</v>
+      </c>
+      <c r="R8" t="n">
+        <v>4</v>
+      </c>
+      <c r="S8" t="n">
+        <v>365</v>
+      </c>
       <c r="T8" t="n">
         <v>4365</v>
       </c>
@@ -1325,11 +1355,19 @@
       <c r="X8" t="n">
         <v>6488377</v>
       </c>
+      <c r="Y8" t="n">
+        <v>0</v>
+      </c>
       <c r="Z8" t="inlineStr">
         <is>
           <t>POLICIAMENTO OSTENSIVO GERAL</t>
         </is>
       </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>POLÍCIA OSTENSIVA</t>
+        </is>
+      </c>
       <c r="AB8" t="inlineStr">
         <is>
           <t>Acordo Repactuação Rio Doce</t>
@@ -1337,12 +1375,12 @@
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
@@ -1352,17 +1390,7 @@
       </c>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>ALTERAMOS A DISTRIBUIÇÃO DO RECURSO</t>
-        </is>
-      </c>
-      <c r="AG8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
-        </is>
-      </c>
-      <c r="AH8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Acordo Repactuação Rio Doce - N/A - A cadastrar - Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
+          <t xml:space="preserve">Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
         </is>
       </c>
     </row>
@@ -1463,12 +1491,12 @@
       </c>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD9" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE9" t="inlineStr">
@@ -1478,17 +1506,7 @@
       </c>
       <c r="AF9" t="inlineStr">
         <is>
-          <t>Valor da PM ficou a mais do que o final (não autorizado a mudar). Deixei o valor total da base Mariana e o resto no geral</t>
-        </is>
-      </c>
-      <c r="AG9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
-        </is>
-      </c>
-      <c r="AH9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Acordo Repactuação Rio Doce - N/A - A cadastrar - Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
+          <t xml:space="preserve">Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
         </is>
       </c>
     </row>
@@ -1589,12 +1607,12 @@
       </c>
       <c r="AC10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD10" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE10" t="inlineStr">
@@ -1602,14 +1620,9 @@
           <t>Fomento à cadeia produtiva da cultura e turismo</t>
         </is>
       </c>
-      <c r="AG10" t="inlineStr">
-        <is>
-          <t>Fomento à cadeia produtiva da cultura e turismo</t>
-        </is>
-      </c>
-      <c r="AH10" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Fomento à cadeia produtiva da cultura e turismo</t>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Fomento à cadeia produtiva da cultura e turismo</t>
         </is>
       </c>
     </row>
@@ -1710,12 +1723,12 @@
       </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD11" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE11" t="inlineStr">
@@ -1723,14 +1736,9 @@
           <t>Fomento à cadeia produtiva da cultura e turismo</t>
         </is>
       </c>
-      <c r="AG11" t="inlineStr">
-        <is>
-          <t>Fomento à cadeia produtiva da cultura e turismo</t>
-        </is>
-      </c>
-      <c r="AH11" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Fomento à cadeia produtiva da cultura e turismo</t>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Fomento à cadeia produtiva da cultura e turismo</t>
         </is>
       </c>
     </row>
@@ -1831,7 +1839,7 @@
       </c>
       <c r="AC12" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>Anexo III</t>
         </is>
       </c>
       <c r="AD12" t="n">
@@ -1842,9 +1850,9 @@
           <t>Implantação do Rodoanel da Região Metropolitana de Belo Horizonte</t>
         </is>
       </c>
-      <c r="AH12" t="inlineStr">
-        <is>
-          <t>Acordo Judicial Vale - III - 9288180 - Implantação do Rodoanel da Região Metropolitana de Belo Horizonte</t>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>Acordo Judicial Vale - Anexo III - 9288180 - Implantação do Rodoanel da Região Metropolitana de Belo Horizonte</t>
         </is>
       </c>
     </row>
@@ -1945,33 +1953,22 @@
       </c>
       <c r="AC13" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE13" t="inlineStr">
         <is>
-          <t>Investimentos em infraestrutura nos estados de Minas Gerais (Cooperação Interfederativa)</t>
+          <t>Cooperação Interfederativa de Infraestrutura de Mobilidade</t>
         </is>
       </c>
       <c r="AF13" t="inlineStr">
         <is>
-          <t>Projeto consta em outra minuta;
-Nome do projeto foi alterado conforme mudanças na minuta do capítulo específico</t>
-        </is>
-      </c>
-      <c r="AG13" t="inlineStr">
-        <is>
-          <t>Cooperação Interfederativa de Infraestrutura de Mobilidade</t>
-        </is>
-      </c>
-      <c r="AH13" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - A cadastrar - N/A - Investimentos em infraestrutura nos estados de Minas Gerais (Cooperação Interfederativa)</t>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Cooperação Interfederativa de Infraestrutura de Mobilidade</t>
         </is>
       </c>
     </row>
@@ -2072,7 +2069,7 @@
       </c>
       <c r="AC14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Sem anexo</t>
         </is>
       </c>
       <c r="AD14" t="n">
@@ -2085,12 +2082,7 @@
       </c>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>Não foi o que a gente mandou e a relação receita e despesa por acordo/anexo não vai bater. Supera?</t>
-        </is>
-      </c>
-      <c r="AH14" t="inlineStr">
-        <is>
-          <t>Agenda Integrada - Renova - N/A - 9382040 - Marliéria</t>
+          <t>Agenda Integrada - Renova - Sem anexo - 9382040 - Marliéria</t>
         </is>
       </c>
     </row>
@@ -2191,7 +2183,7 @@
       </c>
       <c r="AC15" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>Anexo III</t>
         </is>
       </c>
       <c r="AD15" t="n">
@@ -2204,12 +2196,7 @@
       </c>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>Não foi o que a gente mandou. No detalhamento de obra colocaram genérico "ACORDO JUDICIAL PARA REPARAÇÃO INTEGRAL RELATIVA AO ROMPIMENTO DAS BARRAGENS B-I, B-IV E B-IV", no município de Brumadinho, talvez pensando na estrada do distrito industrial mas como saber? Foco que das obras ainda pendentes tem obra dessa iniciativa e já com limite definido (ex: Capela Nova-Carandaí)</t>
-        </is>
-      </c>
-      <c r="AH15" t="inlineStr">
-        <is>
-          <t>Acordo Judicial Vale - III - 9288133 - Recuperação de rodovias pavimentadas em pior estado, conforme avaliação técnica do DER-MG/conclusão de corredor logístico estruturante, conforme critérios técnicos da SEINFRA</t>
+          <t>Acordo Judicial Vale - Anexo III - 9288133 - Recuperação de rodovias pavimentadas em pior estado, conforme avaliação técnica do DER-MG/conclusão de corredor logístico estruturante, conforme critérios técnicos da SEINFRA</t>
         </is>
       </c>
     </row>
@@ -2310,7 +2297,7 @@
       </c>
       <c r="AC16" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>Anexo III</t>
         </is>
       </c>
       <c r="AD16" t="n">
@@ -2323,12 +2310,7 @@
       </c>
       <c r="AF16" t="inlineStr">
         <is>
-          <t>Não teve detalhamento de obras, só um nome genérico "Acordo". Sugestão de deixar no Construção que é onde vai ter as maiores obras (Pintópolis, Ponte São Francisco, Ponte Manga)</t>
-        </is>
-      </c>
-      <c r="AH16" t="inlineStr">
-        <is>
-          <t>Acordo Judicial Vale - III - 9288132 - Construção de pontes em São Francisco, Manga e São Romão sobre o Rio São Francisco</t>
+          <t>Acordo Judicial Vale - Anexo III - 9288132 - Construção de pontes em São Francisco, Manga e São Romão sobre o Rio São Francisco</t>
         </is>
       </c>
     </row>
@@ -2429,7 +2411,7 @@
       </c>
       <c r="AC17" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>Anexo III</t>
         </is>
       </c>
       <c r="AD17" t="n">
@@ -2440,9 +2422,9 @@
           <t>Implantação do Rodoanel da Região Metropolitana de Belo Horizonte</t>
         </is>
       </c>
-      <c r="AH17" t="inlineStr">
-        <is>
-          <t>Acordo Judicial Vale - III - 9288180 - Implantação do Rodoanel da Região Metropolitana de Belo Horizonte</t>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>Acordo Judicial Vale - Anexo III - 9288180 - Implantação do Rodoanel da Região Metropolitana de Belo Horizonte</t>
         </is>
       </c>
     </row>
@@ -2543,12 +2525,12 @@
       </c>
       <c r="AC18" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE18" t="inlineStr">
@@ -2558,17 +2540,7 @@
       </c>
       <c r="AF18" t="inlineStr">
         <is>
-          <t>Não constam na minuta, nomes de projetos enviados pela SES que ainda não constam no caítulo específico</t>
-        </is>
-      </c>
-      <c r="AG18" t="inlineStr">
-        <is>
-          <t>Fortalecimento da Atenção Primária à Saúde</t>
-        </is>
-      </c>
-      <c r="AH18" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - A cadastrar - N/A - Fortalecimento da Atenção Primária à Saúde</t>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Fortalecimento da Atenção Primária à Saúde</t>
         </is>
       </c>
     </row>
@@ -2669,12 +2641,12 @@
       </c>
       <c r="AC19" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD19" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE19" t="inlineStr">
@@ -2684,17 +2656,7 @@
       </c>
       <c r="AF19" t="inlineStr">
         <is>
-          <t>Não constam na minuta, nomes de projetos enviados pela SES que ainda não constam no caítulo específico</t>
-        </is>
-      </c>
-      <c r="AG19" t="inlineStr">
-        <is>
-          <t>Fortalecimento da Rede de Atenção Psicossocial</t>
-        </is>
-      </c>
-      <c r="AH19" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - A cadastrar - N/A - Fortalecimento da Rede de Atenção Psicossocial</t>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Fortalecimento da Rede de Atenção Psicossocial</t>
         </is>
       </c>
     </row>
@@ -2795,12 +2757,12 @@
       </c>
       <c r="AC20" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD20" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE20" t="inlineStr">
@@ -2808,14 +2770,9 @@
           <t>Planejamento e execução de estratégias para adequação dos municípios mineiros às mudanças climáticas, visando à redução de riscos potenciais</t>
         </is>
       </c>
-      <c r="AG20" t="inlineStr">
-        <is>
-          <t>Planejamento e execução de estratégias para adequação dos municípios mineiros às mudanças climáticas, visando à redução de riscos potenciais</t>
-        </is>
-      </c>
-      <c r="AH20" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Planejamento e execução de estratégias para adequação dos municípios mineiros às mudanças climáticas, visando à redução de riscos potenciais</t>
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Planejamento e execução de estratégias para adequação dos municípios mineiros às mudanças climáticas, visando à redução de riscos potenciais</t>
         </is>
       </c>
     </row>
@@ -2916,27 +2873,22 @@
       </c>
       <c r="AC21" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD21" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE21" t="inlineStr">
         <is>
-          <t>Revitalização aquática da Bacia Hidrográfica do rio Doce, a partir do mapeamento de áreas estratégicas para revitalização e conservação da fauna e flora aquáticas, em especial áreas de cabeceiras, tributários e rotas de piracema, e execução de ações como zoneamento pesqueiro; desassoreamento; reconformação de calhas de rios; renaturalização de leitos de rios; reintrodução de espécies aquáticas ameaçadas; educação ambiental, dentre outras ações baseadas na natureza para a revitalização intracalha do rio Doce e seus tributários</t>
-        </is>
-      </c>
-      <c r="AG21" t="inlineStr">
-        <is>
           <t>Revitalização aquática da bacia hidrográfica do rio Doce, a partir do mapeamento de áreas estratégicas para revitalização e conservação da fauna e flora aquáticas, em especial áreas de cabeceiras, tributários e rotas de piracema, e execução de ações como zoneamento pesqueiro; desassoreamento; reconformação de calhas de rios; renaturalização de leitos de rios; reintrodução de espécies aquáticas ameaçadas; educação ambiental, dentre outras ações baseadas na natureza para a revitalização intracalha do rio Doce e seus tributários</t>
         </is>
       </c>
-      <c r="AH21" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Revitalização aquática da Bacia Hidrográfica do rio Doce, a partir do mapeamento de áreas estratégicas para revitalização e conservação da fauna e flora aquáticas, em especial áreas de cabeceiras, tributários e rotas de piracema, e execução de ações como zoneamento pesqueiro; desassoreamento; reconformação de calhas de rios; renaturalização de leitos de rios; reintrodução de espécies aquáticas ameaçadas; educação ambiental, dentre outras ações baseadas na natureza para a revitalização intracalha do rio Doce e seus tributários</t>
+      <c r="AF21" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Revitalização aquática da bacia hidrográfica do rio Doce, a partir do mapeamento de áreas estratégicas para revitalização e conservação da fauna e flora aquáticas, em especial áreas de cabeceiras, tributários e rotas de piracema, e execução de ações como zoneamento pesqueiro; desassoreamento; reconformação de calhas de rios; renaturalização de leitos de rios; reintrodução de espécies aquáticas ameaçadas; educação ambiental, dentre outras ações baseadas na natureza para a revitalização intracalha do rio Doce e seus tributários</t>
         </is>
       </c>
     </row>
@@ -3037,12 +2989,12 @@
       </c>
       <c r="AC22" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD22" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE22" t="inlineStr">
@@ -3050,14 +3002,9 @@
           <t>Recuperação da vegetação nativa na bacia hidrográfica do rio Doce, com prioridade às áreas de mata ripária, por meio de projetos de reflorestamento, pagamento de serviços ambientais, mapeamento do uso de solo e investimento tecnológico para monitoramento da vegetação nativa e sua recuperação</t>
         </is>
       </c>
-      <c r="AG22" t="inlineStr">
-        <is>
-          <t>Recuperação da vegetação nativa na bacia hidrográfica do rio Doce, com prioridade às áreas de mata ripária, por meio de projetos de reflorestamento, pagamento de serviços ambientais, mapeamento do uso de solo e investimento tecnológico para monitoramento da vegetação nativa e sua recuperação</t>
-        </is>
-      </c>
-      <c r="AH22" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Recuperação da vegetação nativa na bacia hidrográfica do rio Doce, com prioridade às áreas de mata ripária, por meio de projetos de reflorestamento, pagamento de serviços ambientais, mapeamento do uso de solo e investimento tecnológico para monitoramento da vegetação nativa e sua recuperação</t>
+      <c r="AF22" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Recuperação da vegetação nativa na bacia hidrográfica do rio Doce, com prioridade às áreas de mata ripária, por meio de projetos de reflorestamento, pagamento de serviços ambientais, mapeamento do uso de solo e investimento tecnológico para monitoramento da vegetação nativa e sua recuperação</t>
         </is>
       </c>
     </row>
@@ -3158,12 +3105,12 @@
       </c>
       <c r="AC23" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD23" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE23" t="inlineStr">
@@ -3171,14 +3118,9 @@
           <t>Consolidação de unidades de conservação estaduais na bacia hidrográfica do rio Doce, a partir do investimento e custeio de suas estruturas e serviços prestados, de acordo com seus objetivos de criação; criação, se necessário, de nova(s) unidade(s) de conservação na bacia hidrográfica do rio Doce de acordo com mapeamento de áreas prioritárias para conservação; realização de atividades de prevenção e combate a incêndios e regularização fundiária das unidades de conservação</t>
         </is>
       </c>
-      <c r="AG23" t="inlineStr">
-        <is>
-          <t>Consolidação de unidades de conservação estaduais na bacia hidrográfica do rio Doce, a partir do investimento e custeio de suas estruturas e serviços prestados, de acordo com seus objetivos de criação; criação, se necessário, de nova(s) unidade(s) de conservação na bacia hidrográfica do rio Doce de acordo com mapeamento de áreas prioritárias para conservação; realização de atividades de prevenção e combate a incêndios e regularização fundiária das unidades de conservação</t>
-        </is>
-      </c>
-      <c r="AH23" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Consolidação de unidades de conservação estaduais na bacia hidrográfica do rio Doce, a partir do investimento e custeio de suas estruturas e serviços prestados, de acordo com seus objetivos de criação; criação, se necessário, de nova(s) unidade(s) de conservação na bacia hidrográfica do rio Doce de acordo com mapeamento de áreas prioritárias para conservação; realização de atividades de prevenção e combate a incêndios e regularização fundiária das unidades de conservação</t>
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Consolidação de unidades de conservação estaduais na bacia hidrográfica do rio Doce, a partir do investimento e custeio de suas estruturas e serviços prestados, de acordo com seus objetivos de criação; criação, se necessário, de nova(s) unidade(s) de conservação na bacia hidrográfica do rio Doce de acordo com mapeamento de áreas prioritárias para conservação; realização de atividades de prevenção e combate a incêndios e regularização fundiária das unidades de conservação</t>
         </is>
       </c>
     </row>
@@ -3279,27 +3221,22 @@
       </c>
       <c r="AC24" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD24" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE24" t="inlineStr">
         <is>
-          <t>Fortalecimento da política pública de gestão do manejo da fauna silvestre, de acordo com mapeamento de necessidades a ser detalhado, a partir de ações como da estruturação e custeio dos serviços prestados porelos Cetras que atendam à bacia hidrográfica do rio Doce; contratação de serviços veterinários especializados; construção de viveiros em áreas de parceiros para a reabilitação e conservação da fauna</t>
-        </is>
-      </c>
-      <c r="AG24" t="inlineStr">
-        <is>
           <t>Fortalecimento da política pública de gestão do manejo da fauna silvestre, de acordo com mapeamento de necessidades a ser detalhado, a partir de ações como da estruturação e custeio dos serviços prestados pelos Cetras que atendam à bacia hidrográfica do rio Doce; contratação de serviços veterinários especializados; construção de viveiros em áreas de parceiros para a reabilitação e conservação da fauna</t>
         </is>
       </c>
-      <c r="AH24" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Fortalecimento da política pública de gestão do manejo da fauna silvestre, de acordo com mapeamento de necessidades a ser detalhado, a partir de ações como da estruturação e custeio dos serviços prestados porelos Cetras que atendam à bacia hidrográfica do rio Doce; contratação de serviços veterinários especializados; construção de viveiros em áreas de parceiros para a reabilitação e conservação da fauna</t>
+      <c r="AF24" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Fortalecimento da política pública de gestão do manejo da fauna silvestre, de acordo com mapeamento de necessidades a ser detalhado, a partir de ações como da estruturação e custeio dos serviços prestados pelos Cetras que atendam à bacia hidrográfica do rio Doce; contratação de serviços veterinários especializados; construção de viveiros em áreas de parceiros para a reabilitação e conservação da fauna</t>
         </is>
       </c>
     </row>
@@ -3400,27 +3337,22 @@
       </c>
       <c r="AC25" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD25" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE25" t="inlineStr">
         <is>
-          <t>Aquisição de materiais, equipamentos e capacitações para modernização da fiscalização ambiental e viabilização da implantação de serviços de inteligência em fiscalização na Secretaria Estadual do Meio Ambiente de Minas Gerais</t>
-        </is>
-      </c>
-      <c r="AG25" t="inlineStr">
-        <is>
           <t>Aquisição de materiais, equipamentos e capacitações para modernização da fiscalização ambiental e viabilização da implantação de serviços de inteligência em fiscalização no Sistema Estadual do Meio Ambiente de Minas Gerais</t>
         </is>
       </c>
-      <c r="AH25" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Aquisição de materiais, equipamentos e capacitações para modernização da fiscalização ambiental e viabilização da implantação de serviços de inteligência em fiscalização na Secretaria Estadual do Meio Ambiente de Minas Gerais</t>
+      <c r="AF25" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Aquisição de materiais, equipamentos e capacitações para modernização da fiscalização ambiental e viabilização da implantação de serviços de inteligência em fiscalização no Sistema Estadual do Meio Ambiente de Minas Gerais</t>
         </is>
       </c>
     </row>
@@ -3506,7 +3438,7 @@
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> MODERNIZAÇÃO E ESTRUTURAÇÃO DO CORPO DE BOMBEIROS MILITAR DE MINAS GERAIS</t>
+          <t>MODERNIZAÇÃO E ESTRUTURAÇÃO DO CORPO DE BOMBEIROS MILITAR DE MINAS GERAIS</t>
         </is>
       </c>
       <c r="AA26" t="inlineStr">
@@ -3521,32 +3453,22 @@
       </c>
       <c r="AC26" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD26" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG </t>
+          <t>Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
         </is>
       </c>
       <c r="AF26" t="inlineStr">
         <is>
-          <t>Valor do CBBMG ficou a menos do que o final (não autorizado a mudar). Deixei o valor total da base Mariana e o resto no geral</t>
-        </is>
-      </c>
-      <c r="AG26" t="inlineStr">
-        <is>
-          <t>Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
-        </is>
-      </c>
-      <c r="AH26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Acordo Repactuação Rio Doce - N/A - A cadastrar - Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG </t>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
         </is>
       </c>
     </row>
@@ -3594,6 +3516,24 @@
       <c r="M27" t="n">
         <v>1</v>
       </c>
+      <c r="N27" t="n">
+        <v>10377</v>
+      </c>
+      <c r="O27" t="n">
+        <v>6</v>
+      </c>
+      <c r="P27" t="n">
+        <v>182</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>52</v>
+      </c>
+      <c r="R27" t="n">
+        <v>4</v>
+      </c>
+      <c r="S27" t="n">
+        <v>120</v>
+      </c>
       <c r="T27" t="n">
         <v>4120</v>
       </c>
@@ -3609,9 +3549,17 @@
       <c r="X27" t="n">
         <v>4621003</v>
       </c>
+      <c r="Y27" t="n">
+        <v>0</v>
+      </c>
       <c r="Z27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> MODERNIZAÇÃO E ESTRUTURAÇÃO DO CORPO DE BOMBEIROS MILITAR DE MINAS GERAIS</t>
+          <t>MODERNIZAÇÃO E ESTRUTURAÇÃO DO CORPO DE BOMBEIROS MILITAR DE MINAS GERAIS</t>
+        </is>
+      </c>
+      <c r="AA27" t="inlineStr">
+        <is>
+          <t>PROMOÇÃO DE DEFESA CIVIL</t>
         </is>
       </c>
       <c r="AB27" t="inlineStr">
@@ -3621,32 +3569,22 @@
       </c>
       <c r="AC27" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD27" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG </t>
+          <t>Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
         </is>
       </c>
       <c r="AF27" t="inlineStr">
         <is>
-          <t>Valor do CBBMG ficou a menos do que o final (não autorizado a mudar). Deixei o valor total da base Mariana e o resto no geral</t>
-        </is>
-      </c>
-      <c r="AG27" t="inlineStr">
-        <is>
-          <t>Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
-        </is>
-      </c>
-      <c r="AH27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Acordo Repactuação Rio Doce - N/A - A cadastrar - Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG </t>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
         </is>
       </c>
     </row>
@@ -3732,7 +3670,7 @@
       </c>
       <c r="Z28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> MODERNIZAÇÃO E ESTRUTURAÇÃO DO CORPO DE BOMBEIROS MILITAR DE MINAS GERAIS</t>
+          <t>MODERNIZAÇÃO E ESTRUTURAÇÃO DO CORPO DE BOMBEIROS MILITAR DE MINAS GERAIS</t>
         </is>
       </c>
       <c r="AA28" t="inlineStr">
@@ -3747,12 +3685,12 @@
       </c>
       <c r="AC28" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD28" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE28" t="inlineStr">
@@ -3762,17 +3700,7 @@
       </c>
       <c r="AF28" t="inlineStr">
         <is>
-          <t>Valor do CBBMG ficou a menos do que o final (não autorizado a mudar). Deixei o valor total da base Mariana e o resto no geral</t>
-        </is>
-      </c>
-      <c r="AG28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
-        </is>
-      </c>
-      <c r="AH28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Acordo Repactuação Rio Doce - N/A - A cadastrar - Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
+          <t xml:space="preserve">Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
         </is>
       </c>
     </row>
@@ -3873,27 +3801,22 @@
       </c>
       <c r="AC29" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD29" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE29" t="inlineStr">
         <is>
-          <t>Fomento da política de prevenção à violência doméstica e atenção à mulher</t>
-        </is>
-      </c>
-      <c r="AG29" t="inlineStr">
-        <is>
           <t>Promoção, defesa e garantia dos direitos das mulheres e fomento da política de prevenção à violência doméstica e atenção à mulher</t>
         </is>
       </c>
-      <c r="AH29" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Fomento da política de prevenção à violência doméstica e atenção à mulher</t>
+      <c r="AF29" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Promoção, defesa e garantia dos direitos das mulheres e fomento da política de prevenção à violência doméstica e atenção à mulher</t>
         </is>
       </c>
     </row>
@@ -3941,6 +3864,24 @@
       <c r="M30" t="n">
         <v>1</v>
       </c>
+      <c r="N30" t="n">
+        <v>10803</v>
+      </c>
+      <c r="O30" t="n">
+        <v>4</v>
+      </c>
+      <c r="P30" t="n">
+        <v>122</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>148</v>
+      </c>
+      <c r="R30" t="n">
+        <v>2</v>
+      </c>
+      <c r="S30" t="n">
+        <v>79</v>
+      </c>
       <c r="T30" t="n">
         <v>2079</v>
       </c>
@@ -3956,11 +3897,19 @@
       <c r="X30" t="n">
         <v>14032546</v>
       </c>
+      <c r="Y30" t="n">
+        <v>0</v>
+      </c>
       <c r="Z30" t="inlineStr">
         <is>
           <t>APOIO FINANCEIRO E MATERIAL ÀS INSTITUIÇÕES NA PROMOÇÃO DO DESENVOLVIMENTO SOCIAL</t>
         </is>
       </c>
+      <c r="AA30" t="inlineStr">
+        <is>
+          <t>APOIO ÀS POLÍTICAS DE DESENVOLVIMENTO SOCIAL</t>
+        </is>
+      </c>
       <c r="AB30" t="inlineStr">
         <is>
           <t>Acordo Repactuação Rio Doce</t>
@@ -3968,12 +3917,12 @@
       </c>
       <c r="AC30" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD30" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE30" t="inlineStr">
@@ -3981,14 +3930,9 @@
           <t>Fortalecimento do atendimento da rede socioassistencial com execução de um plano de melhorias, que inclua, preferencialmente, construção e reforma de unidades do CRAS e CREAS, contratação de equipe técnica e aquisição de material de consumo de acordo com detalhamento a ser construído prioritariamente</t>
         </is>
       </c>
-      <c r="AG30" t="inlineStr">
-        <is>
-          <t>Fortalecimento do atendimento da rede socioassistencial com execução de um plano de melhorias, que inclua, preferencialmente, construção e reforma de unidades do CRAS e CREAS, contratação de equipe técnica e aquisição de material de consumo de acordo com detalhamento a ser construído prioritariamente</t>
-        </is>
-      </c>
-      <c r="AH30" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Fortalecimento do atendimento da rede socioassistencial com execução de um plano de melhorias, que inclua, preferencialmente, construção e reforma de unidades do CRAS e CREAS, contratação de equipe técnica e aquisição de material de consumo de acordo com detalhamento a ser construído prioritariamente</t>
+      <c r="AF30" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Fortalecimento do atendimento da rede socioassistencial com execução de um plano de melhorias, que inclua, preferencialmente, construção e reforma de unidades do CRAS e CREAS, contratação de equipe técnica e aquisição de material de consumo de acordo com detalhamento a ser construído prioritariamente</t>
         </is>
       </c>
     </row>
@@ -4036,6 +3980,24 @@
       <c r="M31" t="n">
         <v>1</v>
       </c>
+      <c r="N31" t="n">
+        <v>10803</v>
+      </c>
+      <c r="O31" t="n">
+        <v>4</v>
+      </c>
+      <c r="P31" t="n">
+        <v>122</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>148</v>
+      </c>
+      <c r="R31" t="n">
+        <v>2</v>
+      </c>
+      <c r="S31" t="n">
+        <v>79</v>
+      </c>
       <c r="T31" t="n">
         <v>2079</v>
       </c>
@@ -4051,11 +4013,19 @@
       <c r="X31" t="n">
         <v>15470409</v>
       </c>
+      <c r="Y31" t="n">
+        <v>0</v>
+      </c>
       <c r="Z31" t="inlineStr">
         <is>
           <t>APOIO FINANCEIRO E MATERIAL ÀS INSTITUIÇÕES NA PROMOÇÃO DO DESENVOLVIMENTO SOCIAL</t>
         </is>
       </c>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>APOIO ÀS POLÍTICAS DE DESENVOLVIMENTO SOCIAL</t>
+        </is>
+      </c>
       <c r="AB31" t="inlineStr">
         <is>
           <t>Acordo Repactuação Rio Doce</t>
@@ -4063,12 +4033,12 @@
       </c>
       <c r="AC31" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD31" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE31" t="inlineStr">
@@ -4076,14 +4046,9 @@
           <t>Fortalecimento do atendimento da rede socioassistencial com execução de um plano de melhorias, que inclua, preferencialmente, construção e reforma de unidades do CRAS e CREAS, contratação de equipe técnica e aquisição de material de consumo de acordo com detalhamento a ser construído prioritariamente</t>
         </is>
       </c>
-      <c r="AG31" t="inlineStr">
-        <is>
-          <t>Fortalecimento do atendimento da rede socioassistencial com execução de um plano de melhorias, que inclua, preferencialmente, construção e reforma de unidades do CRAS e CREAS, contratação de equipe técnica e aquisição de material de consumo de acordo com detalhamento a ser construído prioritariamente</t>
-        </is>
-      </c>
-      <c r="AH31" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Fortalecimento do atendimento da rede socioassistencial com execução de um plano de melhorias, que inclua, preferencialmente, construção e reforma de unidades do CRAS e CREAS, contratação de equipe técnica e aquisição de material de consumo de acordo com detalhamento a ser construído prioritariamente</t>
+      <c r="AF31" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Fortalecimento do atendimento da rede socioassistencial com execução de um plano de melhorias, que inclua, preferencialmente, construção e reforma de unidades do CRAS e CREAS, contratação de equipe técnica e aquisição de material de consumo de acordo com detalhamento a ser construído prioritariamente</t>
         </is>
       </c>
     </row>
@@ -4131,6 +4096,24 @@
       <c r="M32" t="n">
         <v>1</v>
       </c>
+      <c r="N32" t="n">
+        <v>10803</v>
+      </c>
+      <c r="O32" t="n">
+        <v>4</v>
+      </c>
+      <c r="P32" t="n">
+        <v>122</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>148</v>
+      </c>
+      <c r="R32" t="n">
+        <v>2</v>
+      </c>
+      <c r="S32" t="n">
+        <v>79</v>
+      </c>
       <c r="T32" t="n">
         <v>2079</v>
       </c>
@@ -4146,6 +4129,9 @@
       <c r="X32" t="n">
         <v>6441250</v>
       </c>
+      <c r="Y32" t="n">
+        <v>0</v>
+      </c>
       <c r="Z32" t="inlineStr">
         <is>
           <t>APOIO FINANCEIRO E MATERIAL ÀS INSTITUIÇÕES NA PROMOÇÃO DO DESENVOLVIMENTO SOCIAL</t>
@@ -4158,12 +4144,12 @@
       </c>
       <c r="AC32" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD32" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE32" t="inlineStr">
@@ -4171,14 +4157,9 @@
           <t>Oferta de capacitações continuadas em gestão para os profissionais do SUAS, além do apoio na elaboração e execução do Plano Municipal de Assistência Social</t>
         </is>
       </c>
-      <c r="AG32" t="inlineStr">
-        <is>
-          <t>Oferta de capacitações continuadas em gestão para os profissionais do SUAS, além do apoio na elaboração e execução do Plano Municipal de Assistência Social</t>
-        </is>
-      </c>
-      <c r="AH32" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Oferta de capacitações continuadas em gestão para os profissionais do SUAS, além do apoio na elaboração e execução do Plano Municipal de Assistência Social</t>
+      <c r="AF32" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Oferta de capacitações continuadas em gestão para os profissionais do SUAS, além do apoio na elaboração e execução do Plano Municipal de Assistência Social</t>
         </is>
       </c>
     </row>
@@ -4279,12 +4260,12 @@
       </c>
       <c r="AC33" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD33" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE33" t="inlineStr">
@@ -4292,14 +4273,9 @@
           <t>Disponibilização de microcrédito para financiamento de atividades produtivas, podendo ter o apoio de agentes de crédito facilitadores</t>
         </is>
       </c>
-      <c r="AG33" t="inlineStr">
-        <is>
-          <t>Disponibilização de microcrédito para financiamento de atividades produtivas, podendo ter o apoio de agentes de crédito facilitadores</t>
-        </is>
-      </c>
-      <c r="AH33" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Disponibilização de microcrédito para financiamento de atividades produtivas, podendo ter o apoio de agentes de crédito facilitadores</t>
+      <c r="AF33" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Disponibilização de microcrédito para financiamento de atividades produtivas, podendo ter o apoio de agentes de crédito facilitadores</t>
         </is>
       </c>
     </row>
@@ -4400,12 +4376,12 @@
       </c>
       <c r="AC34" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD34" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE34" t="inlineStr">
@@ -4413,14 +4389,9 @@
           <t>Oferta de cursos de qualificação profissional a partir de estudo de demandas do mercado de trabalho</t>
         </is>
       </c>
-      <c r="AG34" t="inlineStr">
-        <is>
-          <t>Oferta de cursos de qualificação profissional a partir de estudo de demandas do mercado de trabalho</t>
-        </is>
-      </c>
-      <c r="AH34" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Oferta de cursos de qualificação profissional a partir de estudo de demandas do mercado de trabalho</t>
+      <c r="AF34" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Oferta de cursos de qualificação profissional a partir de estudo de demandas do mercado de trabalho</t>
         </is>
       </c>
     </row>
@@ -4521,7 +4492,7 @@
       </c>
       <c r="AC35" t="inlineStr">
         <is>
-          <t>Ressarcimentos e contratações temporárias</t>
+          <t>Item 4.4.10: Ressarcimentos e contratações temporárias</t>
         </is>
       </c>
       <c r="AD35" t="n">
@@ -4534,12 +4505,7 @@
       </c>
       <c r="AF35" t="inlineStr">
         <is>
-          <t>Janela</t>
-        </is>
-      </c>
-      <c r="AH35" t="inlineStr">
-        <is>
-          <t>Acordo Judicial Vale - Ressarcimentos e contratações temporárias - 9288191 - Ressarcimentos de despesas públicas</t>
+          <t>Acordo Judicial Vale - Item 4.4.10: Ressarcimentos e contratações temporárias - 9288191 - Ressarcimentos de despesas públicas</t>
         </is>
       </c>
     </row>
@@ -4640,33 +4606,22 @@
       </c>
       <c r="AC36" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD36" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG </t>
+          <t>Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
         </is>
       </c>
       <c r="AF36" t="inlineStr">
         <is>
-          <t>Valor da PC ficou a mais do que o final (não autorizado a mudar). Deixei o valor total da base Mariana e o resto no geral
-Ajustamos o valor, que estava errado na nossa base. Ainda assim, houve diferença e mantive no fortalecimento</t>
-        </is>
-      </c>
-      <c r="AG36" t="inlineStr">
-        <is>
-          <t>Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
-        </is>
-      </c>
-      <c r="AH36" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Acordo Repactuação Rio Doce - N/A - A cadastrar - Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG </t>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Adequação e equipagem de Bases de Segurança Pública (PMMG, CBMMG e PCMG) no Município de Mariana/MG</t>
         </is>
       </c>
     </row>
@@ -4714,6 +4669,24 @@
       <c r="M37" t="n">
         <v>1</v>
       </c>
+      <c r="N37" t="n">
+        <v>10279</v>
+      </c>
+      <c r="O37" t="n">
+        <v>6</v>
+      </c>
+      <c r="P37" t="n">
+        <v>181</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>32</v>
+      </c>
+      <c r="R37" t="n">
+        <v>4</v>
+      </c>
+      <c r="S37" t="n">
+        <v>60</v>
+      </c>
       <c r="T37" t="n">
         <v>4060</v>
       </c>
@@ -4729,11 +4702,19 @@
       <c r="X37" t="n">
         <v>3087684</v>
       </c>
+      <c r="Y37" t="n">
+        <v>0</v>
+      </c>
       <c r="Z37" t="inlineStr">
         <is>
           <t>GESTÃO DAS UNIDADES POLICIAIS</t>
         </is>
       </c>
+      <c r="AA37" t="inlineStr">
+        <is>
+          <t>INVESTIGAÇÃO</t>
+        </is>
+      </c>
       <c r="AB37" t="inlineStr">
         <is>
           <t>Acordo Repactuação Rio Doce</t>
@@ -4741,12 +4722,12 @@
       </c>
       <c r="AC37" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD37" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE37" t="inlineStr">
@@ -4756,17 +4737,7 @@
       </c>
       <c r="AF37" t="inlineStr">
         <is>
-          <t>Valor da PC ficou a mais do que o final (não autorizado a mudar). Deixei o valor total da base Mariana e o resto no geral</t>
-        </is>
-      </c>
-      <c r="AG37" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
-        </is>
-      </c>
-      <c r="AH37" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Acordo Repactuação Rio Doce - N/A - A cadastrar - Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
+          <t xml:space="preserve">Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
         </is>
       </c>
     </row>
@@ -4867,12 +4838,12 @@
       </c>
       <c r="AC38" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD38" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE38" t="inlineStr">
@@ -4882,17 +4853,7 @@
       </c>
       <c r="AF38" t="inlineStr">
         <is>
-          <t>Valor da PC ficou a mais do que o final (não autorizado a mudar). Deixei o valor total da base Mariana e o resto no geral</t>
-        </is>
-      </c>
-      <c r="AG38" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
-        </is>
-      </c>
-      <c r="AH38" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Acordo Repactuação Rio Doce - N/A - A cadastrar - Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
+          <t xml:space="preserve">Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Fortalecimento da infraestrutura e logística das unidades das forças de segurança </t>
         </is>
       </c>
     </row>
@@ -4993,12 +4954,12 @@
       </c>
       <c r="AC39" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Anexo a definir</t>
         </is>
       </c>
       <c r="AD39" t="inlineStr">
         <is>
-          <t>A cadastrar</t>
+          <t>Instrumento de entrada a cadastrar</t>
         </is>
       </c>
       <c r="AE39" t="inlineStr">
@@ -5006,14 +4967,9 @@
           <t>Criação de fundo de disponibilização de crédito para recuperação econômica de pequenas, médias e grandes empresas dos municípios atingidos, além de fundo garantidor para facilitar o acesso a essa linha de crédito</t>
         </is>
       </c>
-      <c r="AG39" t="inlineStr">
-        <is>
-          <t>Criação de fundo de disponibilização de crédito para recuperação econômica de pequenas, médias e grandes empresas dos municípios atingidos, além de fundo garantidor para facilitar o acesso a essa linha de crédito</t>
-        </is>
-      </c>
-      <c r="AH39" t="inlineStr">
-        <is>
-          <t>Acordo Repactuação Rio Doce - N/A - A cadastrar - Criação de fundo de disponibilização de crédito para recuperação econômica de pequenas, médias e grandes empresas dos municípios atingidos, além de fundo garantidor para facilitar o acesso a essa linha de crédito</t>
+      <c r="AF39" t="inlineStr">
+        <is>
+          <t>Acordo Repactuação Rio Doce - Anexo a definir - Instrumento de entrada a cadastrar - Criação de fundo de disponibilização de crédito para recuperação econômica de pequenas, médias e grandes empresas dos municípios atingidos, além de fundo garantidor para facilitar o acesso a essa linha de crédito</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data package at: 2024-09-26T20:27:39Z
</commit_message>
<xml_diff>
--- a/data/base_qdd_fiscal_fonte_95.xlsx
+++ b/data/base_qdd_fiscal_fonte_95.xlsx
@@ -3508,7 +3508,7 @@
         <v>90</v>
       </c>
       <c r="K27" t="n">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="L27" t="n">
         <v>95</v>
@@ -4135,6 +4135,11 @@
       <c r="Z32" t="inlineStr">
         <is>
           <t>APOIO FINANCEIRO E MATERIAL ÀS INSTITUIÇÕES NA PROMOÇÃO DO DESENVOLVIMENTO SOCIAL</t>
+        </is>
+      </c>
+      <c r="AA32" t="inlineStr">
+        <is>
+          <t>APOIO ÀS POLÍTICAS DE DESENVOLVIMENTO SOCIAL</t>
         </is>
       </c>
       <c r="AB32" t="inlineStr">

</xml_diff>